<commit_message>
Add revised marking sheet for Jungah's thesis
</commit_message>
<xml_diff>
--- a/Supervision/Sohn_Jungah/mae4090-grading-sheet.xlsx
+++ b/Supervision/Sohn_Jungah/mae4090-grading-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Supervision\Sohn_Yungah\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Supervision\Sohn_Jungah\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9C769A-FDA0-4550-942B-4B69AA0D65CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F9FB0-FAFE-4445-A845-D86E64D52245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -1327,139 +1327,139 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="141.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="141.6640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -1474,27 +1474,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="93.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -1509,7 +1509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>29</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="378" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
@@ -1574,10 +1574,10 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>40</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>43</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="218.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>49</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="8" t="str">
         <f>_xlfn.SWITCH(ROUND(SUM(E3*D3,E4*D4,E5*D5,E6*D6,E7*D7,E8*D8,E9*D9,E10*D10),0),0,"F",1,"E",2,"D",3,"C",4,"B",5,"A")</f>
-        <v>A</v>
+        <v>B</v>
       </c>
     </row>
   </sheetData>

</xml_diff>